<commit_message>
server-side record validation bug fix
</commit_message>
<xml_diff>
--- a/tests/integration/WBS.xlsx
+++ b/tests/integration/WBS.xlsx
@@ -1975,9 +1975,6 @@
     <t xml:space="preserve">Atmospheric Flux Systematics</t>
   </si>
   <si>
-    <t xml:space="preserve">2.6 Calibration</t>
-  </si>
-  <si>
     <t xml:space="preserve">SANCHEZ HERRERA, SEBASTIAN</t>
   </si>
   <si>
@@ -2107,6 +2104,9 @@
   </si>
   <si>
     <t xml:space="preserve">LADIEU, DON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.6 Calibration</t>
   </si>
   <si>
     <t xml:space="preserve">2.6.1 Detector Calibration</t>
@@ -3153,11 +3153,11 @@
   </sheetPr>
   <dimension ref="A1:M582"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D333" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O337" activeCellId="0" sqref="O337"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A569" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A578" activeCellId="0" sqref="A578"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
@@ -20734,7 +20734,7 @@
     </row>
     <row r="495" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="8" t="s">
-        <v>650</v>
+        <v>548</v>
       </c>
       <c r="B495" s="9" t="s">
         <v>611</v>
@@ -20749,10 +20749,10 @@
         <v>37</v>
       </c>
       <c r="F495" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="G495" s="12" t="s">
         <v>651</v>
-      </c>
-      <c r="G495" s="12" t="s">
-        <v>652</v>
       </c>
       <c r="H495" s="12" t="s">
         <v>11</v>
@@ -20779,7 +20779,7 @@
         <v>88</v>
       </c>
       <c r="D496" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E496" s="11" t="s">
         <v>37</v>
@@ -20788,7 +20788,7 @@
         <v>126</v>
       </c>
       <c r="G496" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H496" s="12" t="s">
         <v>11</v>
@@ -20824,7 +20824,7 @@
         <v>430</v>
       </c>
       <c r="G497" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H497" s="12" t="s">
         <v>11</v>
@@ -20860,7 +20860,7 @@
         <v>430</v>
       </c>
       <c r="G498" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H498" s="12" t="s">
         <v>11</v>
@@ -20896,7 +20896,7 @@
         <v>98</v>
       </c>
       <c r="G499" s="12" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="H499" s="12" t="s">
         <v>11</v>
@@ -20932,7 +20932,7 @@
         <v>295</v>
       </c>
       <c r="G500" s="12" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H500" s="12" t="s">
         <v>11</v>
@@ -20965,10 +20965,10 @@
         <v>37</v>
       </c>
       <c r="F501" s="28" t="s">
+        <v>658</v>
+      </c>
+      <c r="G501" s="12" t="s">
         <v>659</v>
-      </c>
-      <c r="G501" s="12" t="s">
-        <v>660</v>
       </c>
       <c r="H501" s="12" t="s">
         <v>11</v>
@@ -21001,10 +21001,10 @@
         <v>37</v>
       </c>
       <c r="F502" s="28" t="s">
+        <v>660</v>
+      </c>
+      <c r="G502" s="12" t="s">
         <v>661</v>
-      </c>
-      <c r="G502" s="12" t="s">
-        <v>662</v>
       </c>
       <c r="H502" s="12" t="s">
         <v>11</v>
@@ -21037,10 +21037,10 @@
         <v>58</v>
       </c>
       <c r="F503" s="105" t="s">
+        <v>662</v>
+      </c>
+      <c r="G503" s="12" t="s">
         <v>663</v>
-      </c>
-      <c r="G503" s="12" t="s">
-        <v>664</v>
       </c>
       <c r="H503" s="12" t="s">
         <v>11</v>
@@ -21073,10 +21073,10 @@
         <v>52</v>
       </c>
       <c r="F504" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="G504" s="12" t="s">
         <v>665</v>
-      </c>
-      <c r="G504" s="12" t="s">
-        <v>666</v>
       </c>
       <c r="H504" s="12" t="s">
         <v>11</v>
@@ -21112,7 +21112,7 @@
         <v>207</v>
       </c>
       <c r="G505" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H505" s="12" t="s">
         <v>11</v>
@@ -21148,7 +21148,7 @@
         <v>205</v>
       </c>
       <c r="G506" s="12" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H506" s="12" t="s">
         <v>11</v>
@@ -21181,10 +21181,10 @@
         <v>37</v>
       </c>
       <c r="F507" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="G507" s="12" t="s">
         <v>669</v>
-      </c>
-      <c r="G507" s="12" t="s">
-        <v>670</v>
       </c>
       <c r="H507" s="12" t="s">
         <v>11</v>
@@ -21217,10 +21217,10 @@
         <v>52</v>
       </c>
       <c r="F508" s="12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G508" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H508" s="12" t="s">
         <v>11</v>
@@ -21256,7 +21256,7 @@
         <v>126</v>
       </c>
       <c r="G509" s="12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H509" s="12" t="s">
         <v>11</v>
@@ -21292,7 +21292,7 @@
         <v>126</v>
       </c>
       <c r="G510" s="12" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H510" s="12" t="s">
         <v>11</v>
@@ -21325,10 +21325,10 @@
         <v>52</v>
       </c>
       <c r="F511" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="G511" s="12" t="s">
         <v>674</v>
-      </c>
-      <c r="G511" s="12" t="s">
-        <v>675</v>
       </c>
       <c r="H511" s="12" t="s">
         <v>11</v>
@@ -21361,10 +21361,10 @@
         <v>37</v>
       </c>
       <c r="F512" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="G512" s="12" t="s">
         <v>676</v>
-      </c>
-      <c r="G512" s="12" t="s">
-        <v>677</v>
       </c>
       <c r="H512" s="12" t="s">
         <v>11</v>
@@ -21400,7 +21400,7 @@
         <v>505</v>
       </c>
       <c r="G513" s="12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H513" s="12" t="s">
         <v>11</v>
@@ -21436,7 +21436,7 @@
         <v>505</v>
       </c>
       <c r="G514" s="12" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H514" s="12" t="s">
         <v>11</v>
@@ -21469,10 +21469,10 @@
         <v>37</v>
       </c>
       <c r="F515" s="11" t="s">
+        <v>679</v>
+      </c>
+      <c r="G515" s="12" t="s">
         <v>680</v>
-      </c>
-      <c r="G515" s="12" t="s">
-        <v>681</v>
       </c>
       <c r="H515" s="12" t="s">
         <v>11</v>
@@ -21505,10 +21505,10 @@
         <v>37</v>
       </c>
       <c r="F516" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G516" s="12" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H516" s="12" t="s">
         <v>11</v>
@@ -21541,10 +21541,10 @@
         <v>37</v>
       </c>
       <c r="F517" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G517" s="12" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H517" s="12" t="s">
         <v>11</v>
@@ -21580,7 +21580,7 @@
         <v>511</v>
       </c>
       <c r="G518" s="12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H518" s="12" t="s">
         <v>11</v>
@@ -21613,10 +21613,10 @@
         <v>52</v>
       </c>
       <c r="F519" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G519" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H519" s="12" t="s">
         <v>11</v>
@@ -21652,7 +21652,7 @@
         <v>565</v>
       </c>
       <c r="G520" s="12" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H520" s="12" t="s">
         <v>11</v>
@@ -21688,7 +21688,7 @@
         <v>138</v>
       </c>
       <c r="G521" s="12" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H521" s="12" t="s">
         <v>11</v>
@@ -21721,10 +21721,10 @@
         <v>37</v>
       </c>
       <c r="F522" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="G522" s="12" t="s">
         <v>686</v>
-      </c>
-      <c r="G522" s="12" t="s">
-        <v>687</v>
       </c>
       <c r="H522" s="12" t="s">
         <v>11</v>
@@ -21760,7 +21760,7 @@
         <v>291</v>
       </c>
       <c r="G523" s="12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H523" s="12" t="s">
         <v>11</v>
@@ -21796,7 +21796,7 @@
         <v>291</v>
       </c>
       <c r="G524" s="12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H524" s="12" t="s">
         <v>11</v>
@@ -21882,7 +21882,7 @@
         <v>548</v>
       </c>
       <c r="B527" s="106" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C527" s="23" t="s">
         <v>15</v>
@@ -21897,7 +21897,7 @@
         <v>550</v>
       </c>
       <c r="G527" s="12" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H527" s="12" t="s">
         <v>10</v>
@@ -21918,7 +21918,7 @@
         <v>548</v>
       </c>
       <c r="B528" s="9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C528" s="32" t="s">
         <v>15</v>
@@ -21953,7 +21953,7 @@
         <v>548</v>
       </c>
       <c r="B529" s="106" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C529" s="23" t="s">
         <v>15</v>
@@ -21977,7 +21977,7 @@
         <v>548</v>
       </c>
       <c r="B530" s="9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C530" s="32" t="s">
         <v>88</v>
@@ -22006,7 +22006,7 @@
         <v>548</v>
       </c>
       <c r="B531" s="44" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C531" s="108" t="s">
         <v>147</v>
@@ -22042,7 +22042,7 @@
         <v>548</v>
       </c>
       <c r="B532" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C532" s="23" t="s">
         <v>15</v>
@@ -22054,7 +22054,7 @@
         <v>253</v>
       </c>
       <c r="F532" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G532" s="12" t="s">
         <v>556</v>
@@ -22078,7 +22078,7 @@
         <v>548</v>
       </c>
       <c r="B533" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C533" s="32" t="s">
         <v>15</v>
@@ -22113,7 +22113,7 @@
         <v>548</v>
       </c>
       <c r="B534" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C534" s="23" t="s">
         <v>88</v>
@@ -22137,7 +22137,7 @@
         <v>548</v>
       </c>
       <c r="B535" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C535" s="32" t="s">
         <v>88</v>
@@ -22166,7 +22166,7 @@
         <v>548</v>
       </c>
       <c r="B536" s="44" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C536" s="45" t="s">
         <v>147</v>
@@ -22233,7 +22233,7 @@
     </row>
     <row r="538" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B538" s="79" t="s">
         <v>694</v>
@@ -22269,7 +22269,7 @@
     </row>
     <row r="539" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B539" s="79" t="s">
         <v>694</v>
@@ -22305,7 +22305,7 @@
     </row>
     <row r="540" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B540" s="9" t="s">
         <v>694</v>
@@ -22341,7 +22341,7 @@
     </row>
     <row r="541" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B541" s="9" t="s">
         <v>694</v>
@@ -22377,7 +22377,7 @@
     </row>
     <row r="542" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B542" s="9" t="s">
         <v>694</v>
@@ -22413,7 +22413,7 @@
     </row>
     <row r="543" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B543" s="9" t="s">
         <v>694</v>
@@ -22449,7 +22449,7 @@
     </row>
     <row r="544" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B544" s="9" t="s">
         <v>694</v>
@@ -22485,7 +22485,7 @@
     </row>
     <row r="545" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B545" s="9" t="s">
         <v>694</v>
@@ -22521,7 +22521,7 @@
     </row>
     <row r="546" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B546" s="9" t="s">
         <v>694</v>
@@ -22557,7 +22557,7 @@
     </row>
     <row r="547" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B547" s="9" t="s">
         <v>694</v>
@@ -22593,7 +22593,7 @@
     </row>
     <row r="548" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B548" s="9" t="s">
         <v>694</v>
@@ -22629,7 +22629,7 @@
     </row>
     <row r="549" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B549" s="9" t="s">
         <v>694</v>
@@ -22665,7 +22665,7 @@
     </row>
     <row r="550" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B550" s="9" t="s">
         <v>694</v>
@@ -22700,7 +22700,7 @@
     </row>
     <row r="551" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B551" s="9" t="s">
         <v>694</v>
@@ -22736,7 +22736,7 @@
     </row>
     <row r="552" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B552" s="9" t="s">
         <v>694</v>
@@ -22772,7 +22772,7 @@
     </row>
     <row r="553" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B553" s="9" t="s">
         <v>694</v>
@@ -22808,7 +22808,7 @@
     </row>
     <row r="554" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B554" s="9" t="s">
         <v>694</v>
@@ -22844,7 +22844,7 @@
     </row>
     <row r="555" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B555" s="9" t="s">
         <v>694</v>
@@ -22880,7 +22880,7 @@
     </row>
     <row r="556" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B556" s="9" t="s">
         <v>694</v>
@@ -22916,7 +22916,7 @@
     </row>
     <row r="557" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B557" s="9" t="s">
         <v>694</v>
@@ -22952,7 +22952,7 @@
     </row>
     <row r="558" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B558" s="9" t="s">
         <v>694</v>
@@ -22988,7 +22988,7 @@
     </row>
     <row r="559" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B559" s="9" t="s">
         <v>694</v>
@@ -23024,7 +23024,7 @@
     </row>
     <row r="560" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B560" s="9" t="s">
         <v>694</v>
@@ -23060,7 +23060,7 @@
     </row>
     <row r="561" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B561" s="9" t="s">
         <v>694</v>
@@ -23096,7 +23096,7 @@
     </row>
     <row r="562" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B562" s="9" t="s">
         <v>694</v>
@@ -23132,7 +23132,7 @@
     </row>
     <row r="563" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B563" s="9" t="s">
         <v>694</v>
@@ -23168,7 +23168,7 @@
     </row>
     <row r="564" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B564" s="9" t="s">
         <v>694</v>
@@ -23204,7 +23204,7 @@
     </row>
     <row r="565" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B565" s="9" t="s">
         <v>694</v>
@@ -23233,7 +23233,7 @@
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B566" s="44" t="s">
         <v>694</v>
@@ -23269,7 +23269,7 @@
     </row>
     <row r="567" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B567" s="9" t="s">
         <v>727</v>
@@ -23305,7 +23305,7 @@
     </row>
     <row r="568" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B568" s="9" t="s">
         <v>727</v>
@@ -23341,7 +23341,7 @@
     </row>
     <row r="569" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B569" s="9" t="s">
         <v>727</v>
@@ -23377,7 +23377,7 @@
     </row>
     <row r="570" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B570" s="9" t="s">
         <v>727</v>
@@ -23413,7 +23413,7 @@
     </row>
     <row r="571" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B571" s="9" t="s">
         <v>727</v>
@@ -23449,7 +23449,7 @@
     </row>
     <row r="572" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B572" s="9" t="s">
         <v>727</v>
@@ -23485,7 +23485,7 @@
     </row>
     <row r="573" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B573" s="9" t="s">
         <v>727</v>
@@ -23520,7 +23520,7 @@
     </row>
     <row r="574" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B574" s="9" t="s">
         <v>727</v>
@@ -23556,7 +23556,7 @@
     </row>
     <row r="575" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B575" s="9" t="s">
         <v>727</v>
@@ -23592,7 +23592,7 @@
     </row>
     <row r="576" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="8" t="s">
-        <v>548</v>
+        <v>693</v>
       </c>
       <c r="B576" s="9" t="s">
         <v>727</v>
@@ -23628,7 +23628,7 @@
     </row>
     <row r="577" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="8" t="s">
-        <v>548</v>
+        <v>693</v>
       </c>
       <c r="B577" s="9" t="s">
         <v>727</v>
@@ -23664,7 +23664,7 @@
     </row>
     <row r="578" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="8" t="s">
-        <v>548</v>
+        <v>693</v>
       </c>
       <c r="B578" s="9" t="s">
         <v>727</v>
@@ -23700,7 +23700,7 @@
     </row>
     <row r="579" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B579" s="9" t="s">
         <v>727</v>
@@ -23729,7 +23729,7 @@
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="8" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B580" s="44" t="s">
         <v>727</v>
@@ -23765,7 +23765,7 @@
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="111" t="s">
-        <v>650</v>
+        <v>693</v>
       </c>
       <c r="B581" s="112" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
table tooltips; rename a few columns
</commit_message>
<xml_diff>
--- a/tests/integration/WBS.xlsx
+++ b/tests/integration/WBS.xlsx
@@ -37,10 +37,10 @@
     <t xml:space="preserve">Labor Cat.</t>
   </si>
   <si>
-    <t xml:space="preserve">Names</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tasks</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task Description</t>
   </si>
   <si>
     <t xml:space="preserve">Source of Funds (U.S. Only)</t>
@@ -3153,11 +3153,11 @@
   </sheetPr>
   <dimension ref="A1:M582"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A569" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A578" activeCellId="0" sqref="A578"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>

</xml_diff>